<commit_message>
complete a series of TODO
</commit_message>
<xml_diff>
--- a/fs/index.xlsx
+++ b/fs/index.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\gitee\luckyexcel4j\fs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58E338BB-5AB4-422B-B228-7EFF972A9CC6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F932E36-4BD5-49D1-A122-13B2DA320CDB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3000" yWindow="3000" windowWidth="19200" windowHeight="10510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2520" yWindow="4250" windowWidth="19200" windowHeight="10510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -191,7 +191,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -276,14 +276,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -292,7 +306,13 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="7" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -305,11 +325,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="7" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment textRotation="45"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -607,10 +628,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -618,8 +639,8 @@
     <col min="3" max="3" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1">
@@ -628,73 +649,74 @@
       <c r="C1">
         <v>1.1000000000000001</v>
       </c>
-      <c r="D1" s="17">
+      <c r="D1" s="11">
         <v>2.2000000000000002</v>
       </c>
-      <c r="E1" s="16">
+      <c r="E1" s="10">
         <v>3.3</v>
       </c>
-      <c r="F1" s="18">
+      <c r="F1" s="12">
         <v>4.4000000000000004</v>
       </c>
-      <c r="G1" s="19">
+      <c r="G1" s="13">
         <v>5.5</v>
       </c>
-      <c r="H1" s="20">
+      <c r="H1" s="14">
         <v>6.6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C2" s="9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C2" s="8">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C3" s="4"/>
-      <c r="D3" s="10">
+    <row r="3" spans="1:9" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C3" s="3"/>
+      <c r="D3" s="9">
         <v>3</v>
       </c>
-      <c r="H3" s="3"/>
-    </row>
-    <row r="4" spans="1:8" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="D4" s="5"/>
-      <c r="E4" s="11">
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="1:9" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="D4" s="4"/>
+      <c r="E4" s="16">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F5" s="1">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F5" s="15">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E7" s="12"/>
-      <c r="F7" s="13"/>
-    </row>
-    <row r="8" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="8" t="s">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E7" s="17"/>
+      <c r="F7" s="18"/>
+      <c r="I7" s="22"/>
+    </row>
+    <row r="8" spans="1:9" ht="48.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="15"/>
-    </row>
-    <row r="10" spans="1:8" ht="14.5" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
+      <c r="D8" s="4"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="20"/>
+    </row>
+    <row r="10" spans="1:9" ht="14.5" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="20.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:9" ht="20.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="E7:F8"/>

</xml_diff>